<commit_message>
Unsure about the desorption results, mass balance violated
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
+++ b/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
@@ -471,7 +471,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[m]"/>
+    <numFmt numFmtId="164" formatCode="[m]"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -657,7 +657,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,7 +690,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -822,11 +821,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="501341712"/>
-        <c:axId val="501339360"/>
+        <c:axId val="391676984"/>
+        <c:axId val="391680904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="501341712"/>
+        <c:axId val="391676984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,12 +882,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501339360"/>
+        <c:crossAx val="391680904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="501339360"/>
+        <c:axId val="391680904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +944,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501341712"/>
+        <c:crossAx val="391676984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5121,10 +5120,10 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomRight" activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Another round of edits, as well as additional analysis of namont kinetic data
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
+++ b/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
@@ -816,7 +816,7 @@
                   <c:v>0.49280272850001111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3552375099985434</c:v>
+                  <c:v>0.4739107033915938</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.48737807490377466</c:v>
@@ -840,11 +840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408667688"/>
-        <c:axId val="408668472"/>
+        <c:axId val="385302152"/>
+        <c:axId val="385297448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408667688"/>
+        <c:axId val="385302152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,12 +901,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408668472"/>
+        <c:crossAx val="385297448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="408668472"/>
+        <c:axId val="385297448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,7 +963,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408667688"/>
+        <c:crossAx val="385302152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5142,7 +5142,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S17" sqref="S17"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6664,7 +6664,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6783,32 +6783,32 @@
         <v>138</v>
       </c>
       <c r="B3">
-        <f>AVERAGE('Bottle Results'!Q5:Q7)</f>
-        <v>1.3552375099985434</v>
+        <f>AVERAGE('Bottle Results'!Q5,'Bottle Results'!Q7)</f>
+        <v>0.4739107033915938</v>
       </c>
       <c r="C3">
-        <f>_xlfn.STDEV.S('Bottle Results'!Q5:Q7)</f>
-        <v>1.526560033704331</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!Q5,'Bottle Results'!Q7)</f>
+        <v>1.8693120197463428E-2</v>
       </c>
       <c r="D3">
-        <f>AVERAGE('Bottle Results'!U5:U7)</f>
-        <v>3305.5968272979794</v>
+        <f>AVERAGE('Bottle Results'!U5,'Bottle Results'!U7)</f>
+        <v>6203.9965487825075</v>
       </c>
       <c r="E3">
-        <f>_xlfn.STDEV.S('Bottle Results'!U5:U7)</f>
-        <v>5020.1812958564369</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!U5,'Bottle Results'!U7)</f>
+        <v>10.715107282799851</v>
       </c>
       <c r="F3">
-        <f>AVERAGE('Bottle Results'!S5:S7)</f>
-        <v>235.06007175857499</v>
+        <f>AVERAGE('Bottle Results'!S5,'Bottle Results'!S7)</f>
+        <v>235.06007175857502</v>
       </c>
       <c r="G3">
-        <f>AVERAGE('Bottle Results'!W5:W7)</f>
-        <v>0.42345056739773418</v>
+        <f>AVERAGE('Bottle Results'!W5,'Bottle Results'!W7)</f>
+        <v>0.79838740801613595</v>
       </c>
       <c r="H3">
-        <f>_xlfn.STDEV.S('Bottle Results'!W5:W7)</f>
-        <v>0.64943400309697286</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!W5,'Bottle Results'!W7)</f>
+        <v>7.9524863825714311E-3</v>
       </c>
       <c r="I3">
         <f>AVERAGE('Bottle Results'!D5:D7)</f>

</xml_diff>

<commit_message>
Further edits, cleared tracked changes, cannot resolve NaMont desorption mass balance
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
+++ b/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
@@ -840,11 +840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385302152"/>
-        <c:axId val="385297448"/>
+        <c:axId val="474001104"/>
+        <c:axId val="473996792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385302152"/>
+        <c:axId val="474001104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,12 +901,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385297448"/>
+        <c:crossAx val="473996792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385297448"/>
+        <c:axId val="473996792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,7 +963,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385302152"/>
+        <c:crossAx val="474001104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1572,16 +1572,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4570,7 +4570,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5139,10 +5139,10 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6664,7 +6664,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Organizing figures and tables for draft
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
+++ b/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -840,11 +840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492791032"/>
-        <c:axId val="492785544"/>
+        <c:axId val="212535048"/>
+        <c:axId val="212535832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="492791032"/>
+        <c:axId val="212535048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,12 +901,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492785544"/>
+        <c:crossAx val="212535832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492785544"/>
+        <c:axId val="212535832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,7 +963,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492791032"/>
+        <c:crossAx val="212535048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1874,8 +1874,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1976,20 +1976,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.25" style="2" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.75" style="2" customWidth="1"/>
     <col min="7" max="7" width="12" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="18.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.25" style="2" customWidth="1"/>
+    <col min="9" max="10" width="18.75" style="2" customWidth="1"/>
     <col min="11" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -3816,8 +3816,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4569,19 +4569,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5147,30 +5147,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -6663,14 +6663,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6751,6 +6751,10 @@
         <f>AVERAGE('Bottle Results'!W2:W4)</f>
         <v>0.79035030287655239</v>
       </c>
+      <c r="H2">
+        <f>_xlfn.STDEV.S('Bottle Results'!W2:W4)</f>
+        <v>3.0956501771457158E-3</v>
+      </c>
       <c r="I2">
         <f>AVERAGE('Bottle Results'!D2:D4)</f>
         <v>7.0533333333333337</v>

</xml_diff>

<commit_message>
Final edits to draft
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
+++ b/Sorption Experiments/RaMont_pH7/RaMont_pH7_Kinetics_NoScript.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Sorption Experiments\RaMont_pH7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mache\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Sorption Experiments\RaMont_pH7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[m]"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,6 +587,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -664,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -716,6 +723,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5190,11 +5200,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z2" sqref="Z2"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6888,381 +6898,384 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="9.140625" style="27"/>
+    <col min="11" max="11" width="20.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="27"/>
+    <col min="15" max="15" width="23.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="27">
         <v>90</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="27" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="27">
         <f>AVERAGE('Bottle Results'!Q2:Q4)</f>
         <v>0.49280272850001111</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!Q2:Q4)</f>
         <v>7.2766375277932257E-3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="27">
         <f>AVERAGE('Bottle Results'!U2:U4)</f>
         <v>5294.5368624163357</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!U2:U4)</f>
         <v>37.09574631107894</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="27">
         <f>AVERAGE('Bottle Results'!S2:S4)</f>
         <v>206.34929577464791</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="27">
         <f>AVERAGE('Bottle Results'!W2:W4)</f>
         <v>0.76118031968560906</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!W2:W4)</f>
         <v>3.5263689660177118E-3</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="27">
         <f>AVERAGE('Bottle Results'!D2:D4)</f>
         <v>7.0533333333333337</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!D2:D4)</f>
         <v>2.5166114784235766E-2</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="28">
         <f>AVERAGE('Bottle Results'!Z2:Z4)</f>
         <v>0.12175925926082225</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="29">
         <f>AVERAGE('Bottle Results'!E2:E4)</f>
         <v>2.9666666666666664E-2</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="27">
         <f>B6*(100-P1)+D6*L6</f>
         <v>148.84619344013095</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="27" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="27">
         <f>AVERAGE('Bottle Results'!Q5,'Bottle Results'!Q7)</f>
         <v>0.4739107033915938</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!Q5,'Bottle Results'!Q7)</f>
         <v>1.8693120197463428E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="27">
         <f>AVERAGE('Bottle Results'!U5,'Bottle Results'!U7)</f>
         <v>5254.8151569641523</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!U5,'Bottle Results'!U7)</f>
         <v>0.37865467969396022</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="27">
         <f>AVERAGE('Bottle Results'!S5,'Bottle Results'!S7)</f>
         <v>206.34929577464791</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="27">
         <f>AVERAGE('Bottle Results'!W5,'Bottle Results'!W7)</f>
         <v>0.77033568173203404</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!W5,'Bottle Results'!W7)</f>
         <v>9.0589697082746543E-3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="27">
         <f>AVERAGE('Bottle Results'!D5:D7)</f>
         <v>6.9899999999999993</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!D5:D7)</f>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="28">
         <f>AVERAGE('Bottle Results'!Z5:Z7)</f>
         <v>0.25995370370461995</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="29">
         <f>AVERAGE('Bottle Results'!E5:E7)</f>
         <v>3.043333333333333E-2</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="27">
         <f>100</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="27">
         <f>AVERAGE('Bottle Results'!Q8:Q10)</f>
         <v>0.48737807490377466</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!Q8:Q10)</f>
         <v>2.8428336036186521E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="27">
         <f>AVERAGE('Bottle Results'!U8:U10)</f>
         <v>5277.2160944556308</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!U8:U10)</f>
         <v>16.75890915533158</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="27">
         <f>AVERAGE('Bottle Results'!S8:S10)</f>
         <v>206.34929577464791</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="27">
         <f>AVERAGE('Bottle Results'!W8:W10)</f>
         <v>0.76380918913528273</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!W8:W10)</f>
         <v>1.3776803031706442E-2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="27">
         <f>AVERAGE('Bottle Results'!D8:D10)</f>
         <v>7.0233333333333334</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!D8:D10)</f>
         <v>2.3094010767585053E-2</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="28">
         <f>AVERAGE('Bottle Results'!Z8:Z10)</f>
         <v>1.0004629629644721</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="29">
         <f>AVERAGE('Bottle Results'!E8:E10)</f>
         <v>2.9866666666666666E-2</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="27">
         <f>P3*B7</f>
         <v>222.22333791620693</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="27">
         <f>AVERAGE('Bottle Results'!Q11:Q13)</f>
         <v>0.54139351575777994</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!Q11:Q13)</f>
         <v>0.10139268183274636</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="27">
         <f>AVERAGE('Bottle Results'!U11:U13)</f>
         <v>5123.1253873893811</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!U11:U13)</f>
         <v>269.65011857204559</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="27">
         <f>AVERAGE('Bottle Results'!S11:S13)</f>
         <v>206.34929577464791</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="27">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
         <v>0.7376324868348324</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
         <v>4.9136432209333385E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="27">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
         <v>6.996666666666667</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!D11:D13)</f>
         <v>2.0816659994660883E-2</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="28">
         <f>AVERAGE('Bottle Results'!Z11:Z13)</f>
         <v>10.796990740743544</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="29">
         <f>AVERAGE('Bottle Results'!E11:E13)</f>
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="27">
         <f>AVERAGE('Bottle Results'!Q14:Q16)</f>
         <v>0.6385629273728789</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!Q14:Q16)</f>
         <v>5.4642132775437717E-2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="27">
         <f>AVERAGE('Bottle Results'!U14:U16)</f>
         <v>4829.1716666577004</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!U14:U16)</f>
         <v>113.70432787624559</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="27">
         <f>AVERAGE('Bottle Results'!S14:S16)</f>
         <v>206.34929577464791</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="27">
         <f>AVERAGE('Bottle Results'!W14:W16)</f>
         <v>0.69054271545939871</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!W14:W16)</f>
         <v>2.6480406715374452E-2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="27">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
         <v>6.9900000000000011</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!D14:D16)</f>
         <v>3.6055512754639987E-2</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="28">
         <f>AVERAGE('Bottle Results'!Z14:Z16)</f>
         <v>10.784953703706075</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="29">
         <f>AVERAGE('Bottle Results'!E14:E16)</f>
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="27">
         <f>AVERAGE('Bottle Results'!Q17:Q19)</f>
         <v>2.2222333791620694</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!Q17:Q19)</f>
         <v>0.12544534831751561</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="27">
         <f>AVERAGE('Bottle Results'!U17:U19)</f>
         <v>-2701.3813592473684</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!U17:U19)</f>
         <v>284.51080832697806</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="27">
         <f>AVERAGE('Bottle Results'!S17:S19)</f>
         <v>142.49300303736004</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="27">
         <f>AVERAGE('Bottle Results'!W17:W19)</f>
         <v>-0.55931822375175166</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!W17:W19)</f>
         <v>5.7056743851220865E-2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="27">
         <f>AVERAGE('Bottle Results'!D17:D19)</f>
         <v>7</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="27">
         <f>_xlfn.STDEV.S('Bottle Results'!D17:D19)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="28">
         <f>AVERAGE('Bottle Results'!Z17:Z19)</f>
         <v>0.99027777777761605</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="29">
         <f>AVERAGE('Bottle Results'!E17:E19)</f>
         <v>2.9499999999999998E-2</v>
       </c>

</xml_diff>